<commit_message>
Added wrapper classes to make the Emotiv SDK more manageable. Connection is possible, but not sure how to create events off connecting or plugging in quite yet. Today's goals, connect automatically when Bluetooth dongle is plugged in.
</commit_message>
<xml_diff>
--- a/Documents/Time Logs/TimeLog_EricCarlson.xlsx
+++ b/Documents/Time Logs/TimeLog_EricCarlson.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcarlson\Documents\School\Quarter 7\Capstone\Eric Carlson - Mind Control\Documents\Time Logs\Week 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcarlson\Documents\School\Quarter 7\Capstone\Eric Carlson - Mind Control\Documents\Time Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="16">
   <si>
     <t>Monday</t>
   </si>
@@ -71,6 +71,15 @@
   </si>
   <si>
     <t>Emotiv Research</t>
+  </si>
+  <si>
+    <t>Connecting to Emotiv Headset</t>
+  </si>
+  <si>
+    <t>Creating Wrapper Classes for Emotiv API</t>
+  </si>
+  <si>
+    <t>Coding with/Studying Emotiv API</t>
   </si>
 </sst>
 </file>
@@ -425,17 +434,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -460,10 +469,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>0.14583333333333334</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="B3" s="1">
-        <v>0.1875</v>
+        <v>0.6875</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -474,10 +483,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>0.26041666666666669</v>
+        <v>0.76041666666666663</v>
       </c>
       <c r="B4" s="1">
-        <v>0.29166666666666669</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -488,10 +497,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>0.41666666666666669</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="B5" s="1">
-        <v>0.47916666666666669</v>
+        <v>0.97916666666666663</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -539,28 +548,57 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>3</v>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.96875</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <f>SUM(D11:D14)</f>
+        <v>6.25</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -577,60 +615,107 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="2" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="2" t="s">
+    <row r="35" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="2" t="s">
+    <row r="39" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="3" t="s">
+    <row r="43" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Program can now detect dongle insertion. Wire up has been made to support Create/Load Profile functions. Expanded upon wrapper class. Re-factored convoluted event chain on dongle insert detection.
</commit_message>
<xml_diff>
--- a/Documents/Time Logs/TimeLog_EricCarlson.xlsx
+++ b/Documents/Time Logs/TimeLog_EricCarlson.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="19">
   <si>
     <t>Monday</t>
   </si>
@@ -80,6 +80,15 @@
   </si>
   <si>
     <t>Coding with/Studying Emotiv API</t>
+  </si>
+  <si>
+    <t>Coding - Recognizing Dongle Insertion</t>
+  </si>
+  <si>
+    <t>Coding - Wire up for Create/Load Profiles</t>
+  </si>
+  <si>
+    <t>Today's Total</t>
   </si>
 </sst>
 </file>
@@ -147,11 +156,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
@@ -434,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,37 +521,51 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D7">
-        <f>SUM(D3:D6)</f>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <f ca="1">SUM(D3:D6)</f>
         <v>3.25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
+    <row r="8" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>3</v>
+    <row r="9" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>0.34375</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>0.75</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>0.34375</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="B11" s="1">
-        <v>0.375</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -550,177 +576,224 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>0.54166666666666663</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="B12" s="1">
-        <v>0.57291666666666663</v>
+        <v>0.625</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D12">
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>0.57291666666666663</v>
+        <v>0.82291666666666663</v>
       </c>
       <c r="B13" s="1">
-        <v>0.625</v>
+        <v>0.96875</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D13">
-        <v>1.25</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>0.82291666666666663</v>
-      </c>
-      <c r="B14" s="1">
-        <v>0.96875</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
+      <c r="A14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
       <c r="D14">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D15">
-        <f>SUM(D11:D14)</f>
+        <f>SUM(D10:D13)</f>
         <v>6.25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
+    <row r="16" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>3</v>
+    <row r="17" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <v>2.5</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19">
         <v>0.5</v>
       </c>
-      <c r="B19" s="1">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19">
-        <v>2.5</v>
-      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="B20" s="1">
+      <c r="A20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20">
+        <f>SUM(D18:D19)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B24" s="1">
         <v>0.625</v>
       </c>
-      <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="2" t="s">
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26">
+        <f>SUM(D24:D25)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="2" t="s">
+    <row r="28" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="2" t="s">
+    <row r="33" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D43" s="3" t="s">
+    <row r="37" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A26:C26"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
The new project files in the Source folder are follow along tutorials for learning XNA. I'm fairly new to XNA, so I thought it best to show a product of all the time I am spending on learning XNA. Once XNA is learned, most of the files created throughout the week will be useable in the new XNA project since they are mostly .NET classes, not classes specific to WPF.
</commit_message>
<xml_diff>
--- a/Documents/Time Logs/TimeLog_EricCarlson.xlsx
+++ b/Documents/Time Logs/TimeLog_EricCarlson.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="22">
   <si>
     <t>Monday</t>
   </si>
@@ -89,6 +89,15 @@
   </si>
   <si>
     <t>Today's Total</t>
+  </si>
+  <si>
+    <t>Tutorial Coding with XNA</t>
+  </si>
+  <si>
+    <t>Research - Learned XNA is preferable over WPF</t>
+  </si>
+  <si>
+    <t>This Week's Total Hours</t>
   </si>
 </sst>
 </file>
@@ -156,12 +165,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -446,17 +461,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -748,49 +763,101 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="2" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32">
+        <f>SUM(D30:D31)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="2" t="s">
+    <row r="35" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>3</v>
+    <row r="39" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47">
+        <f>SUM(D3:D5,D10,D11,D12,D13,D18,D19,D24,D25,D30,D31)</f>
+        <v>23.5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A47:C47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>